<commit_message>
fixed chart according to requierments & added some formulas
</commit_message>
<xml_diff>
--- a/src/Excel_zaliczenie_2023_I_termin.xlsx
+++ b/src/Excel_zaliczenie_2023_I_termin.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pawgr\Documents\repos\excel-learning\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Git Repo\excel-learning\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC88B58-2A83-4A20-92CB-EB29B84F864E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A212E9-E4F8-49CE-ADCE-12AC0540EFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kolejność działań" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="183">
   <si>
     <t>Oprocentowanie</t>
   </si>
@@ -854,6 +854,12 @@
   </si>
   <si>
     <t>Check</t>
+  </si>
+  <si>
+    <t>Data końcowa</t>
+  </si>
+  <si>
+    <t>Data początkowa</t>
   </si>
 </sst>
 </file>
@@ -944,7 +950,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1020,12 +1026,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1192,7 +1192,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1224,6 +1223,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1260,24 +1265,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1329,18 +1327,34 @@
     <c:floor>
       <c:thickness val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="accent1"/>
+        </a:solidFill>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
-        <a:sp3d/>
+        <a:sp3d>
+          <a:contourClr>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:contourClr>
+        </a:sp3d>
       </c:spPr>
     </c:floor>
     <c:sideWall>
       <c:thickness val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="90000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -1351,7 +1365,11 @@
     <c:backWall>
       <c:thickness val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="90000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -1365,10 +1383,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12360695538057742"/>
-          <c:y val="0.13008311461067368"/>
-          <c:w val="0.62692169728783897"/>
-          <c:h val="0.34620115193934092"/>
+          <c:x val="0.11951375734406854"/>
+          <c:y val="0.11041705666007809"/>
+          <c:w val="0.67876855140074455"/>
+          <c:h val="0.55815679249230576"/>
         </c:manualLayout>
       </c:layout>
       <c:bar3DChart>
@@ -1782,6 +1800,7 @@
         <c:axId val="1758062992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1798,18 +1817,14 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="bg2">
-                <a:lumMod val="10000"/>
-              </a:schemeClr>
-            </a:solidFill>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1836,6 +1851,7 @@
         <c:crossAx val="1758062032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:serAx>
         <c:axId val="1748270736"/>
@@ -1878,9 +1894,17 @@
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -1929,7 +1953,9 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="bg1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -2565,15 +2591,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>108858</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>48986</xdr:rowOff>
+      <xdr:colOff>908</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>182336</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>21772</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2866,48 +2892,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="9.84375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A2" s="38" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="41"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I10" s="9">
         <f>(1.5/(2.3/4.1))+(((1.2+1)^0.5)/2)*(12.3/((4.5+2)^2-1))</f>
         <v>2.895050598366204</v>
@@ -2927,172 +2953,172 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:AG30"/>
   <sheetViews>
-    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.3828125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="33" width="4.3046875" customWidth="1"/>
+    <col min="13" max="33" width="4.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="44" t="s">
+    <row r="2" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="L2" s="45" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="L2" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="45"/>
-      <c r="S2" s="45"/>
-      <c r="T2" s="45"/>
-      <c r="U2" s="45"/>
-      <c r="V2" s="45"/>
-      <c r="W2" s="45"/>
-      <c r="X2" s="45"/>
-      <c r="Y2" s="45"/>
-      <c r="Z2" s="45"/>
-      <c r="AA2" s="45"/>
-      <c r="AB2" s="45"/>
-      <c r="AC2" s="45"/>
-      <c r="AD2" s="45"/>
-      <c r="AE2" s="45"/>
-      <c r="AF2" s="45"/>
-      <c r="AG2" s="45"/>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.4">
-      <c r="A3" s="44"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
-      <c r="V3" s="45"/>
-      <c r="W3" s="45"/>
-      <c r="X3" s="45"/>
-      <c r="Y3" s="45"/>
-      <c r="Z3" s="45"/>
-      <c r="AA3" s="45"/>
-      <c r="AB3" s="45"/>
-      <c r="AC3" s="45"/>
-      <c r="AD3" s="45"/>
-      <c r="AE3" s="45"/>
-      <c r="AF3" s="45"/>
-      <c r="AG3" s="45"/>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.4">
-      <c r="A4" s="44"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="45"/>
-      <c r="T4" s="45"/>
-      <c r="U4" s="45"/>
-      <c r="V4" s="45"/>
-      <c r="W4" s="45"/>
-      <c r="X4" s="45"/>
-      <c r="Y4" s="45"/>
-      <c r="Z4" s="45"/>
-      <c r="AA4" s="45"/>
-      <c r="AB4" s="45"/>
-      <c r="AC4" s="45"/>
-      <c r="AD4" s="45"/>
-      <c r="AE4" s="45"/>
-      <c r="AF4" s="45"/>
-      <c r="AG4" s="45"/>
-    </row>
-    <row r="5" spans="1:33" ht="4.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="44"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="45"/>
-      <c r="X5" s="45"/>
-      <c r="Y5" s="45"/>
-      <c r="Z5" s="45"/>
-      <c r="AA5" s="45"/>
-      <c r="AB5" s="45"/>
-      <c r="AC5" s="45"/>
-      <c r="AD5" s="45"/>
-      <c r="AE5" s="45"/>
-      <c r="AF5" s="45"/>
-      <c r="AG5" s="45"/>
-    </row>
-    <row r="6" spans="1:33" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="44"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="48"/>
+      <c r="V2" s="48"/>
+      <c r="W2" s="48"/>
+      <c r="X2" s="48"/>
+      <c r="Y2" s="48"/>
+      <c r="Z2" s="48"/>
+      <c r="AA2" s="48"/>
+      <c r="AB2" s="48"/>
+      <c r="AC2" s="48"/>
+      <c r="AD2" s="48"/>
+      <c r="AE2" s="48"/>
+      <c r="AF2" s="48"/>
+      <c r="AG2" s="48"/>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A3" s="47"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="48"/>
+      <c r="V3" s="48"/>
+      <c r="W3" s="48"/>
+      <c r="X3" s="48"/>
+      <c r="Y3" s="48"/>
+      <c r="Z3" s="48"/>
+      <c r="AA3" s="48"/>
+      <c r="AB3" s="48"/>
+      <c r="AC3" s="48"/>
+      <c r="AD3" s="48"/>
+      <c r="AE3" s="48"/>
+      <c r="AF3" s="48"/>
+      <c r="AG3" s="48"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="48"/>
+      <c r="Y4" s="48"/>
+      <c r="Z4" s="48"/>
+      <c r="AA4" s="48"/>
+      <c r="AB4" s="48"/>
+      <c r="AC4" s="48"/>
+      <c r="AD4" s="48"/>
+      <c r="AE4" s="48"/>
+      <c r="AF4" s="48"/>
+      <c r="AG4" s="48"/>
+    </row>
+    <row r="5" spans="1:33" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="47"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="48"/>
+      <c r="S5" s="48"/>
+      <c r="T5" s="48"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="48"/>
+      <c r="W5" s="48"/>
+      <c r="X5" s="48"/>
+      <c r="Y5" s="48"/>
+      <c r="Z5" s="48"/>
+      <c r="AA5" s="48"/>
+      <c r="AB5" s="48"/>
+      <c r="AC5" s="48"/>
+      <c r="AD5" s="48"/>
+      <c r="AE5" s="48"/>
+      <c r="AF5" s="48"/>
+      <c r="AG5" s="48"/>
+    </row>
+    <row r="6" spans="1:33" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>0</v>
       </c>
@@ -3106,12 +3132,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B9" s="5">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="43"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="46"/>
       <c r="E9" s="6">
         <v>20000</v>
       </c>
@@ -3180,16 +3206,16 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="39"/>
+    <row r="10" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="42"/>
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="24">
         <f>E9*$B$9</f>
         <v>1340</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="25">
         <f>E9+D10</f>
         <v>21340</v>
       </c>
@@ -3281,16 +3307,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="40"/>
+    <row r="11" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="43"/>
       <c r="C11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="24">
         <f>E10*$B$9</f>
         <v>1429.78</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="25">
         <f>E10+D11</f>
         <v>22769.78</v>
       </c>
@@ -3382,16 +3408,16 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="40"/>
+    <row r="12" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="43"/>
       <c r="C12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="24">
         <f>E11*$B$9</f>
         <v>1525.5752600000001</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="25">
         <f>E11+D12</f>
         <v>24295.35526</v>
       </c>
@@ -3484,16 +3510,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="41"/>
+    <row r="13" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="44"/>
       <c r="C13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="24">
         <f>E12*$B$9</f>
         <v>1627.7888024200001</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="25">
         <f>E12+D13</f>
         <v>25923.14406242</v>
       </c>
@@ -3585,7 +3611,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D14" s="2"/>
       <c r="L14" s="19">
         <v>4</v>
@@ -3675,7 +3701,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L15" s="19">
         <v>5</v>
       </c>
@@ -3764,7 +3790,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J16" s="1"/>
       <c r="L16" s="19">
         <v>6</v>
@@ -3854,7 +3880,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L17" s="19">
         <v>7</v>
       </c>
@@ -3943,7 +3969,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L18" s="19">
         <v>8</v>
       </c>
@@ -4032,7 +4058,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L19" s="19">
         <v>9</v>
       </c>
@@ -4121,7 +4147,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="20" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L20" s="19">
         <v>10</v>
       </c>
@@ -4210,7 +4236,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L21" s="19">
         <v>11</v>
       </c>
@@ -4299,7 +4325,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="22" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L22" s="19">
         <v>12</v>
       </c>
@@ -4388,7 +4414,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="23" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L23" s="19">
         <v>13</v>
       </c>
@@ -4477,7 +4503,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="24" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L24" s="19">
         <v>14</v>
       </c>
@@ -4566,7 +4592,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="25" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L25" s="19">
         <v>15</v>
       </c>
@@ -4655,7 +4681,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="26" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L26" s="19">
         <v>16</v>
       </c>
@@ -4744,7 +4770,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="27" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L27" s="19">
         <v>17</v>
       </c>
@@ -4833,7 +4859,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="28" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L28" s="19">
         <v>18</v>
       </c>
@@ -4922,7 +4948,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="29" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L29" s="19">
         <v>19</v>
       </c>
@@ -5011,7 +5037,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="30" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="12:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L30" s="19">
         <v>20</v>
       </c>
@@ -5119,35 +5145,35 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="46" t="s">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A3" s="46"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="49"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
       <c r="H3" s="10"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B5" s="16" t="s">
         <v>8</v>
       </c>
@@ -5168,78 +5194,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:AH43"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="38" t="s">
+    <row r="2" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
       <c r="O2" s="10"/>
       <c r="P2" s="17"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="10"/>
       <c r="S2" s="10"/>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.4">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.4">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A4" s="41"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
       <c r="O4" s="10"/>
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" s="12"/>
       <c r="B6" s="13">
         <f>-PI()</f>
@@ -5374,7 +5400,7 @@
         <v>3.560471674068431</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" s="14">
         <f>-PI()</f>
         <v>-3.1415926535897931</v>
@@ -5512,7 +5538,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A8" s="14">
         <f t="shared" ref="A8:A39" si="3">A7+PI()/15</f>
         <v>-2.9321531433504737</v>
@@ -5650,7 +5676,7 @@
         <v>-0.97814760073380569</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A9" s="14">
         <f t="shared" si="3"/>
         <v>-2.7227136331111543</v>
@@ -5788,7 +5814,7 @@
         <v>-0.91354545764260098</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A10" s="14">
         <f t="shared" si="3"/>
         <v>-2.5132741228718349</v>
@@ -5926,7 +5952,7 @@
         <v>-0.80901699437494767</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A11" s="14">
         <f t="shared" si="3"/>
         <v>-2.3038346126325155</v>
@@ -6064,7 +6090,7 @@
         <v>-0.66913060635885857</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A12" s="14">
         <f t="shared" si="3"/>
         <v>-2.0943951023931962</v>
@@ -6202,7 +6228,7 @@
         <v>-0.50000000000000056</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A13" s="14">
         <f t="shared" si="3"/>
         <v>-1.8849555921538765</v>
@@ -6340,7 +6366,7 @@
         <v>-0.30901699437494801</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A14" s="14">
         <f t="shared" si="3"/>
         <v>-1.6755160819145569</v>
@@ -6478,7 +6504,7 @@
         <v>-0.104528463267654</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A15" s="14">
         <f t="shared" si="3"/>
         <v>-1.4660765716752373</v>
@@ -6616,7 +6642,7 @@
         <v>0.10452846326765301</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A16" s="14">
         <f t="shared" si="3"/>
         <v>-1.2566370614359177</v>
@@ -6754,7 +6780,7 @@
         <v>0.30901699437494706</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A17" s="14">
         <f t="shared" si="3"/>
         <v>-1.0471975511965981</v>
@@ -6892,7 +6918,7 @@
         <v>0.49999999999999972</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A18" s="14">
         <f t="shared" si="3"/>
         <v>-0.83775804095727857</v>
@@ -7030,7 +7056,7 @@
         <v>0.6691306063588579</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A19" s="14">
         <f t="shared" si="3"/>
         <v>-0.62831853071795907</v>
@@ -7168,7 +7194,7 @@
         <v>0.80901699437494723</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A20" s="14">
         <f t="shared" si="3"/>
         <v>-0.41887902047863956</v>
@@ -7303,7 +7329,7 @@
         <v>0.91354545764260076</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A21" s="14">
         <f t="shared" si="3"/>
         <v>-0.20943951023932003</v>
@@ -7441,7 +7467,7 @@
         <v>0.97814760073380558</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A22" s="14">
         <f t="shared" si="3"/>
         <v>-4.9960036108132044E-16</v>
@@ -7579,7 +7605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A23" s="14">
         <f t="shared" si="3"/>
         <v>0.20943951023931903</v>
@@ -7717,7 +7743,7 @@
         <v>0.9781476007338058</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A24" s="14">
         <f t="shared" si="3"/>
         <v>0.41887902047863856</v>
@@ -7855,7 +7881,7 @@
         <v>0.91354545764260109</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A25" s="14">
         <f t="shared" si="3"/>
         <v>0.62831853071795807</v>
@@ -7993,7 +8019,7 @@
         <v>0.80901699437494778</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A26" s="14">
         <f t="shared" si="3"/>
         <v>0.83775804095727757</v>
@@ -8131,7 +8157,7 @@
         <v>0.66913060635885868</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A27" s="14">
         <f t="shared" si="3"/>
         <v>1.0471975511965972</v>
@@ -8269,7 +8295,7 @@
         <v>0.50000000000000044</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A28" s="14">
         <f t="shared" si="3"/>
         <v>1.2566370614359168</v>
@@ -8407,7 +8433,7 @@
         <v>0.3090169943749479</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A29" s="14">
         <f t="shared" si="3"/>
         <v>1.4660765716752364</v>
@@ -8545,7 +8571,7 @@
         <v>0.1045284632676539</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A30" s="14">
         <f t="shared" si="3"/>
         <v>1.675516081914556</v>
@@ -8683,7 +8709,7 @@
         <v>-0.10452846326765311</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A31" s="14">
         <f t="shared" si="3"/>
         <v>1.8849555921538756</v>
@@ -8821,7 +8847,7 @@
         <v>-0.30901699437494712</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A32" s="14">
         <f t="shared" si="3"/>
         <v>2.0943951023931953</v>
@@ -8959,7 +8985,7 @@
         <v>-0.49999999999999978</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A33" s="14">
         <f t="shared" si="3"/>
         <v>2.3038346126325147</v>
@@ -9097,7 +9123,7 @@
         <v>-0.6691306063588579</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A34" s="14">
         <f t="shared" si="3"/>
         <v>2.513274122871834</v>
@@ -9235,7 +9261,7 @@
         <v>-0.80901699437494712</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A35" s="14">
         <f t="shared" si="3"/>
         <v>2.7227136331111534</v>
@@ -9373,7 +9399,7 @@
         <v>-0.91354545764260064</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A36" s="14">
         <f t="shared" si="3"/>
         <v>2.9321531433504728</v>
@@ -9511,7 +9537,7 @@
         <v>-0.97814760073380547</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A37" s="14">
         <f t="shared" si="3"/>
         <v>3.1415926535897922</v>
@@ -9649,7 +9675,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A38" s="14">
         <f t="shared" si="3"/>
         <v>3.3510321638291116</v>
@@ -9787,7 +9813,7 @@
         <v>-0.97814760073380591</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A39" s="14">
         <f t="shared" si="3"/>
         <v>3.560471674068431</v>
@@ -9925,11 +9951,11 @@
         <v>-0.91354545764260142</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.4">
-      <c r="C43" s="47" t="s">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="C43" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="D43" s="47"/>
+      <c r="D43" s="50"/>
       <c r="E43" s="9">
         <f>SUM(Zakres_1,Zakres_2)</f>
         <v>-2.1788576534851769</v>
@@ -9948,69 +9974,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3236FC2C-822A-4192-BFCE-4451E24B65EF}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.3828125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.15234375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A5" s="32" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="48"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="32" t="s">
         <v>79</v>
       </c>
       <c r="D5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A6" s="34" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="34">
         <v>6</v>
       </c>
       <c r="D6" s="9" t="str" cm="1">
@@ -10020,21 +10046,21 @@
       <c r="F6" s="16">
         <v>1</v>
       </c>
-      <c r="G6" s="36" t="s">
+      <c r="G6" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="36" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A7" s="34" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="34">
         <v>2</v>
       </c>
       <c r="D7" s="9" t="str">
@@ -10043,21 +10069,21 @@
       <c r="F7" s="16">
         <v>2</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G7" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="H7" s="37" t="s">
+      <c r="H7" s="36" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A8" s="34" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="34">
         <v>5</v>
       </c>
       <c r="D8" s="9" t="str">
@@ -10066,21 +10092,21 @@
       <c r="F8" s="16">
         <v>3</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="36" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A9" s="34" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="34">
         <v>6</v>
       </c>
       <c r="D9" s="9" t="str">
@@ -10089,21 +10115,21 @@
       <c r="F9" s="16">
         <v>4</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="H9" s="37" t="s">
+      <c r="H9" s="36" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A10" s="34" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="34">
         <v>4</v>
       </c>
       <c r="D10" s="9" t="str">
@@ -10112,21 +10138,21 @@
       <c r="F10" s="16">
         <v>5</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="H10" s="37" t="s">
+      <c r="H10" s="36" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A11" s="34" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="34">
         <v>5</v>
       </c>
       <c r="D11" s="9" t="str">
@@ -10135,147 +10161,147 @@
       <c r="F11" s="16">
         <v>6</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="H11" s="37" t="s">
+      <c r="H11" s="36" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A12" s="34" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="34">
         <v>6</v>
       </c>
       <c r="D12" s="9" t="str">
         <v>cel</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A13" s="34" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="34">
         <v>2</v>
       </c>
       <c r="D13" s="9" t="str">
         <v>dop</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A14" s="34" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="34">
         <v>2</v>
       </c>
       <c r="D14" s="9" t="str">
         <v>dop</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A15" s="34" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="C15" s="35">
+      <c r="C15" s="34">
         <v>5</v>
       </c>
       <c r="D15" s="9" t="str">
         <v>bdb</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A16" s="34" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C16" s="34">
         <v>4</v>
       </c>
       <c r="D16" s="9" t="str">
         <v>db</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A17" s="34" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C17" s="34">
         <v>4</v>
       </c>
       <c r="D17" s="9" t="str">
         <v>db</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A18" s="34" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="C18" s="35">
+      <c r="C18" s="34">
         <v>2</v>
       </c>
       <c r="D18" s="9" t="str">
         <v>dop</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A19" s="34" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="C19" s="35">
+      <c r="C19" s="34">
         <v>6</v>
       </c>
       <c r="D19" s="9" t="str">
         <v>cel</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A20" s="34" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="C20" s="35">
+      <c r="C20" s="34">
         <v>5</v>
       </c>
       <c r="D20" s="9" t="str">
         <v>bdb</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A21" s="34" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="C21" s="35">
+      <c r="C21" s="34">
         <v>5</v>
       </c>
       <c r="D21" s="9" t="str">
@@ -10283,462 +10309,462 @@
       </c>
       <c r="K21" s="18"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A22" s="34" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="35">
+      <c r="C22" s="34">
         <v>2</v>
       </c>
       <c r="D22" s="9" t="str">
         <v>dop</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A23" s="34" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="C23" s="35">
+      <c r="C23" s="34">
         <v>3</v>
       </c>
       <c r="D23" s="9" t="str">
         <v>dst</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A24" s="34" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="C24" s="35">
+      <c r="C24" s="34">
         <v>2</v>
       </c>
       <c r="D24" s="9" t="str">
         <v>dop</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A25" s="34" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="C25" s="35">
+      <c r="C25" s="34">
         <v>2</v>
       </c>
       <c r="D25" s="9" t="str">
         <v>dop</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A26" s="34" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="C26" s="35">
+      <c r="C26" s="34">
         <v>2</v>
       </c>
       <c r="D26" s="9" t="str">
         <v>dop</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A27" s="34" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="C27" s="35">
+      <c r="C27" s="34">
         <v>2</v>
       </c>
       <c r="D27" s="9" t="str">
         <v>dop</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A28" s="34" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="C28" s="35">
+      <c r="C28" s="34">
         <v>1</v>
       </c>
       <c r="D28" s="9" t="str">
         <v>ndst</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A29" s="34" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="C29" s="35">
+      <c r="C29" s="34">
         <v>5</v>
       </c>
       <c r="D29" s="9" t="str">
         <v>bdb</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A30" s="34" t="s">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="C30" s="35">
+      <c r="C30" s="34">
         <v>3</v>
       </c>
       <c r="D30" s="9" t="str">
         <v>dst</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A31" s="34" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="B31" s="34" t="s">
+      <c r="B31" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="C31" s="35">
+      <c r="C31" s="34">
         <v>4</v>
       </c>
       <c r="D31" s="9" t="str">
         <v>db</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A32" s="34" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="C32" s="35">
+      <c r="C32" s="34">
         <v>6</v>
       </c>
       <c r="D32" s="9" t="str">
         <v>cel</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A33" s="34" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="B33" s="34" t="s">
+      <c r="B33" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="C33" s="35">
+      <c r="C33" s="34">
         <v>4</v>
       </c>
       <c r="D33" s="9" t="str">
         <v>db</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A34" s="34" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="C34" s="35">
+      <c r="C34" s="34">
         <v>3</v>
       </c>
       <c r="D34" s="9" t="str">
         <v>dst</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A35" s="34" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="B35" s="34" t="s">
+      <c r="B35" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="C35" s="35">
+      <c r="C35" s="34">
         <v>4</v>
       </c>
       <c r="D35" s="9" t="str">
         <v>db</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A36" s="34" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="B36" s="34" t="s">
+      <c r="B36" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="C36" s="35">
+      <c r="C36" s="34">
         <v>3</v>
       </c>
       <c r="D36" s="9" t="str">
         <v>dst</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A37" s="34" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="B37" s="34" t="s">
+      <c r="B37" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="C37" s="35">
+      <c r="C37" s="34">
         <v>2</v>
       </c>
       <c r="D37" s="9" t="str">
         <v>dop</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A38" s="34" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="B38" s="34" t="s">
+      <c r="B38" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="C38" s="35">
+      <c r="C38" s="34">
         <v>3</v>
       </c>
       <c r="D38" s="9" t="str">
         <v>dst</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A39" s="34" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="B39" s="34" t="s">
+      <c r="B39" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="C39" s="35">
+      <c r="C39" s="34">
         <v>3</v>
       </c>
       <c r="D39" s="9" t="str">
         <v>dst</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A40" s="34" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="B40" s="34" t="s">
+      <c r="B40" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="C40" s="35">
+      <c r="C40" s="34">
         <v>3</v>
       </c>
       <c r="D40" s="9" t="str">
         <v>dst</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A41" s="34" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="B41" s="34" t="s">
+      <c r="B41" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="C41" s="35">
+      <c r="C41" s="34">
         <v>4</v>
       </c>
       <c r="D41" s="9" t="str">
         <v>db</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A42" s="34" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="B42" s="34" t="s">
+      <c r="B42" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="C42" s="35">
+      <c r="C42" s="34">
         <v>4</v>
       </c>
       <c r="D42" s="9" t="str">
         <v>db</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A43" s="34" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="B43" s="34" t="s">
+      <c r="B43" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="C43" s="35">
+      <c r="C43" s="34">
         <v>6</v>
       </c>
       <c r="D43" s="9" t="str">
         <v>cel</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A44" s="34" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="33" t="s">
         <v>164</v>
       </c>
-      <c r="B44" s="34" t="s">
+      <c r="B44" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="C44" s="35">
+      <c r="C44" s="34">
         <v>2</v>
       </c>
       <c r="D44" s="9" t="str">
         <v>dop</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A45" s="34" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="33" t="s">
         <v>165</v>
       </c>
-      <c r="B45" s="34" t="s">
+      <c r="B45" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="C45" s="35">
+      <c r="C45" s="34">
         <v>4</v>
       </c>
       <c r="D45" s="9" t="str">
         <v>db</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A46" s="34" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="B46" s="34" t="s">
+      <c r="B46" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="C46" s="35">
+      <c r="C46" s="34">
         <v>5</v>
       </c>
       <c r="D46" s="9" t="str">
         <v>bdb</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A47" s="34" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="B47" s="34" t="s">
+      <c r="B47" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="C47" s="35">
+      <c r="C47" s="34">
         <v>6</v>
       </c>
       <c r="D47" s="9" t="str">
         <v>cel</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A48" s="34" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="B48" s="34" t="s">
+      <c r="B48" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="C48" s="35">
+      <c r="C48" s="34">
         <v>6</v>
       </c>
       <c r="D48" s="9" t="str">
         <v>cel</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A49" s="34" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="33" t="s">
         <v>173</v>
       </c>
-      <c r="B49" s="34" t="s">
+      <c r="B49" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="C49" s="35">
+      <c r="C49" s="34">
         <v>6</v>
       </c>
       <c r="D49" s="9" t="str">
         <v>cel</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A50" s="34" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" s="33" t="s">
         <v>174</v>
       </c>
-      <c r="B50" s="34" t="s">
+      <c r="B50" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="C50" s="35">
+      <c r="C50" s="34">
         <v>6</v>
       </c>
       <c r="D50" s="9" t="str">
         <v>cel</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A51" s="34" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="B51" s="34" t="s">
+      <c r="B51" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="C51" s="35">
+      <c r="C51" s="34">
         <v>6</v>
       </c>
       <c r="D51" s="9" t="str">
         <v>cel</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A52" s="34" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="B52" s="34" t="s">
+      <c r="B52" s="33" t="s">
         <v>176</v>
       </c>
-      <c r="C52" s="35">
+      <c r="C52" s="34">
         <v>6</v>
       </c>
       <c r="D52" s="9" t="str">
         <v>cel</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A53" s="34" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="B53" s="34" t="s">
+      <c r="B53" s="33" t="s">
         <v>178</v>
       </c>
-      <c r="C53" s="35">
+      <c r="C53" s="34">
         <v>6</v>
       </c>
       <c r="D53" s="9" t="str">
         <v>cel</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A54" s="34" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="B54" s="34" t="s">
+      <c r="B54" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="C54" s="35">
+      <c r="C54" s="34">
         <v>6</v>
       </c>
       <c r="D54" s="9" t="str">
@@ -10758,106 +10784,123 @@
   <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.69140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.3828125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.15234375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="14" max="18" width="14.15234375" customWidth="1"/>
-    <col min="19" max="19" width="16.53515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.36328125" customWidth="1"/>
+    <col min="13" max="13" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="18" width="14.1796875" customWidth="1"/>
+    <col min="19" max="19" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A1" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="M1" s="45" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="M1" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="45"/>
-      <c r="S2" s="45"/>
-      <c r="T2" s="45"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="I4" s="30" t="s">
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" s="48"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="I4" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="45"/>
-      <c r="T4" s="45"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="J4" t="s">
+        <v>182</v>
+      </c>
+      <c r="K4" s="39">
+        <v>40188</v>
+      </c>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="I5" s="31">
+      <c r="B5" s="40">
+        <f>NETWORKDAYS.INTL(K4,K5,1,I5:I7)</f>
+        <v>1590</v>
+      </c>
+      <c r="I5" s="30">
         <v>40219</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="I6" s="31">
+      <c r="J5" t="s">
+        <v>181</v>
+      </c>
+      <c r="K5" s="39">
+        <v>42417</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="I6" s="30">
         <v>40981</v>
       </c>
       <c r="M6" s="22" t="s">
@@ -10884,21 +10927,21 @@
       <c r="T6" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="U6" s="52" t="s">
+      <c r="U6" s="38" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A7" s="45" t="s">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A7" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="I7" s="31">
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="I7" s="30">
         <v>42326</v>
       </c>
       <c r="M7" s="23" t="s">
@@ -10931,14 +10974,14 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A8" s="45"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A8" s="48"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
       <c r="M8" s="23" t="s">
         <v>31</v>
       </c>
@@ -10969,14 +11012,14 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A9" s="45"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A9" s="48"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
       <c r="M9" s="23" t="s">
         <v>32</v>
       </c>
@@ -10999,7 +11042,7 @@
         <v>43</v>
       </c>
       <c r="T9" s="21" t="str">
-        <f t="shared" ref="T8:T9" si="1">IF(OR(SUM(N9:R9,)&gt;85,S9="TAK"),"Uczen zdal na prawo","Uczen niezdal na prawo")</f>
+        <f t="shared" ref="T9" si="1">IF(OR(SUM(N9:R9,)&gt;85,S9="TAK"),"Uczen zdal na prawo","Uczen niezdal na prawo")</f>
         <v>Uczen niezdal na prawo</v>
       </c>
       <c r="U9">
@@ -11007,16 +11050,16 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A10" s="45"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A10" s="48"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
         <v>10</v>
       </c>
@@ -11029,11 +11072,11 @@
       <c r="D12" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="51" t="s">
+      <c r="E12" s="37" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -11052,7 +11095,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -11071,7 +11114,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
@@ -11090,7 +11133,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -11109,7 +11152,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
@@ -11128,7 +11171,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
@@ -11147,7 +11190,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -11166,7 +11209,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
@@ -11185,7 +11228,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
@@ -11204,7 +11247,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
@@ -11223,7 +11266,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>24</v>
       </c>
@@ -11242,7 +11285,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>25</v>
       </c>
@@ -11261,7 +11304,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
@@ -11280,7 +11323,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>27</v>
       </c>
@@ -11299,7 +11342,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>28</v>
       </c>
@@ -11333,162 +11376,162 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{512EC284-8A95-4FD4-AE2D-49341467060B}">
   <dimension ref="A2:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.84375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.15234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.3828125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.84375" customWidth="1"/>
-    <col min="8" max="8" width="9.84375" customWidth="1"/>
+    <col min="1" max="1" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.81640625" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A2" s="50" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A3" s="50"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A4" s="53" t="s">
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="55"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A5" s="53" t="s">
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A6" s="56" t="s">
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A7" s="53" t="s">
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-    </row>
-    <row r="8" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="54" t="s">
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+    </row>
+    <row r="8" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A9" s="55" t="s">
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A10" s="49" t="s">
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A11" s="53" t="s">
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A12" s="53" t="s">
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A13" s="49" t="s">
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="21"/>
       <c r="B15" s="21" t="s">
         <v>47</v>
@@ -11500,157 +11543,157 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="28">
+      <c r="B16" s="27">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C16" s="28">
+      <c r="C16" s="27">
         <v>3.7</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D16" s="27">
         <v>3.7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B17" s="27">
         <v>3.8</v>
       </c>
-      <c r="C17" s="28">
+      <c r="C17" s="27">
         <v>3.4</v>
       </c>
-      <c r="D17" s="28">
+      <c r="D17" s="27">
         <v>3.8</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="28">
+      <c r="B18" s="27">
         <v>3.7</v>
       </c>
-      <c r="C18" s="28">
+      <c r="C18" s="27">
         <v>3.3</v>
       </c>
-      <c r="D18" s="28">
+      <c r="D18" s="27">
         <v>3.7</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="28">
+      <c r="B19" s="27">
         <v>3.9</v>
       </c>
-      <c r="C19" s="28">
+      <c r="C19" s="27">
         <v>3.6</v>
       </c>
-      <c r="D19" s="28">
+      <c r="D19" s="27">
         <v>3.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="28">
+      <c r="B20" s="27">
         <v>3.8</v>
       </c>
-      <c r="C20" s="28">
+      <c r="C20" s="27">
         <v>3.4</v>
       </c>
-      <c r="D20" s="28">
+      <c r="D20" s="27">
         <v>3.4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="28">
+      <c r="B21" s="27">
         <v>3.8</v>
       </c>
-      <c r="C21" s="28">
+      <c r="C21" s="27">
         <v>3.4</v>
       </c>
-      <c r="D21" s="28">
+      <c r="D21" s="27">
         <v>3.4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="29">
+      <c r="B22" s="28">
         <v>3.7</v>
       </c>
-      <c r="C22" s="29">
+      <c r="C22" s="28">
         <v>3.4</v>
       </c>
-      <c r="D22" s="29">
+      <c r="D22" s="28">
         <v>3.7</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="29">
+      <c r="B23" s="28">
         <v>3.7</v>
       </c>
-      <c r="C23" s="29">
+      <c r="C23" s="28">
         <v>3.3</v>
       </c>
-      <c r="D23" s="29">
+      <c r="D23" s="28">
         <v>3.8</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="29">
+      <c r="B24" s="28">
         <v>3.8</v>
       </c>
-      <c r="C24" s="29">
+      <c r="C24" s="28">
         <v>3.2</v>
       </c>
-      <c r="D24" s="29">
+      <c r="D24" s="28">
         <v>3.5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="29">
+      <c r="B25" s="28">
         <v>3.7</v>
       </c>
-      <c r="C25" s="29">
+      <c r="C25" s="28">
         <v>3.1</v>
       </c>
-      <c r="D25" s="29">
+      <c r="D25" s="28">
         <v>3.6</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="29">
+      <c r="B26" s="28">
         <v>3.8</v>
       </c>
-      <c r="C26" s="29">
+      <c r="C26" s="28">
         <v>3.1</v>
       </c>
-      <c r="D26" s="29">
+      <c r="D26" s="28">
         <v>3.4</v>
       </c>
     </row>

</xml_diff>